<commit_message>
Actualizando CU en Listado de Requisitos
</commit_message>
<xml_diff>
--- a/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_LIST_REQ.xlsx
+++ b/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_LIST_REQ.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Requerimientos consolidado" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requerimientos consolidado'!$B$5:$H$5</definedName>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
   <si>
     <t>SUPUESTOS Y RESTRICCIONES (técnicas)</t>
   </si>
@@ -392,6 +391,9 @@
 ▪ Se mostrara una interfaz donde la SA debera ubicar en el menu superior la opcion Informes, debera seleccionar la opcion Gestionar Informes.
 ▪ La SA seleccionara la opcion Gestionar Informes y se mostrara una interface donde se solicitar ingresar el nombre del informe a consultar.
 ▪ Se listaran los registros encontrados, para actualizar ese registro debera ingresar a la opcion ubicada en el lado derecho del registro (icono actualizar).</t>
+  </si>
+  <si>
+    <t>CU11</t>
   </si>
 </sst>
 </file>
@@ -951,11 +953,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1131,7 @@
         <v>94</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>76</v>
@@ -1189,7 +1191,7 @@
         <v>93</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>70</v>
@@ -1222,7 +1224,7 @@
         <v>91</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>77</v>
@@ -1282,7 +1284,7 @@
         <v>99</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>11</v>
@@ -1315,7 +1317,7 @@
         <v>100</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>78</v>
@@ -1375,7 +1377,7 @@
         <v>94</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>81</v>
@@ -1408,7 +1410,7 @@
         <v>95</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>83</v>
@@ -1441,7 +1443,7 @@
         <v>96</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>82</v>
@@ -1501,7 +1503,7 @@
         <v>98</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>16</v>
@@ -1536,590 +1538,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N20"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="53.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="17.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="27" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="7">
-        <v>1</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="10">
-        <v>1</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" ht="231" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" ht="186" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="7">
-        <v>1</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" ht="188.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="10">
-        <v>1</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" ht="187.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" ht="135" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="10">
-        <v>1</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" ht="201.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="7">
-        <v>2</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="2:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="7">
-        <v>2</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="2:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="10">
-        <v>2</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="2:14" ht="214.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="2:14" ht="164.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="7">
-        <v>2</v>
-      </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="K6:K20"/>
-    <mergeCell ref="L6:L20"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J18:J19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizando documentos Trazabilidad Requisitos
</commit_message>
<xml_diff>
--- a/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_LIST_REQ.xlsx
+++ b/METODOLOGIA RUP/PROYECTO STD/02 REQUISITOS/STD_LIST_REQ.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670"/>
@@ -77,12 +77,6 @@
 </t>
   </si>
   <si>
-    <t>La arquitectura lógica deberá considerarse en tres capas
-El software será desarrollado en Java utilizando como Base de datos MySQL.
-El software estará desarrollado  sólo  para ambientes  Web.
-El servidor web a utilizar sera apache tomcat.</t>
-  </si>
-  <si>
     <t>Sistema</t>
   </si>
   <si>
@@ -394,6 +388,12 @@
   </si>
   <si>
     <t>CU11</t>
+  </si>
+  <si>
+    <t>La arquitectura lógica deberá considerarse en tres capas
+El software será desarrollado en PHP utilizando como Base de datos MySQL.
+El software estará desarrollado  sólo  para ambientes  Web.
+El servidor web a utilizar sera apache nginx.</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,6 +581,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,7 +960,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -980,7 +983,7 @@
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1020,10 +1023,10 @@
         <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>6</v>
@@ -1043,7 +1046,7 @@
     </row>
     <row r="6" spans="1:14" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
@@ -1052,19 +1055,19 @@
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" s="7">
         <v>1</v>
@@ -1073,35 +1076,35 @@
         <v>17</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
@@ -1113,28 +1116,28 @@
     </row>
     <row r="8" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8" s="10">
         <v>1</v>
@@ -1146,22 +1149,22 @@
     </row>
     <row r="9" spans="1:14" ht="231" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -1173,28 +1176,28 @@
     </row>
     <row r="10" spans="1:14" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="7">
         <v>1</v>
@@ -1206,28 +1209,28 @@
     </row>
     <row r="11" spans="1:14" ht="188.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" s="10">
         <v>1</v>
@@ -1239,22 +1242,22 @@
     </row>
     <row r="12" spans="1:14" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1266,25 +1269,25 @@
     </row>
     <row r="13" spans="1:14" ht="187.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>11</v>
@@ -1299,28 +1302,28 @@
     </row>
     <row r="14" spans="1:14" ht="171" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J14" s="10">
         <v>1</v>
@@ -1332,22 +1335,22 @@
     </row>
     <row r="15" spans="1:14" ht="206.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="10"/>
@@ -1359,28 +1362,28 @@
     </row>
     <row r="16" spans="1:14" ht="190.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J16" s="7">
         <v>2</v>
@@ -1392,28 +1395,28 @@
     </row>
     <row r="17" spans="2:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J17" s="7">
         <v>2</v>
@@ -1425,28 +1428,28 @@
     </row>
     <row r="18" spans="2:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J18" s="10">
         <v>2</v>
@@ -1458,22 +1461,22 @@
     </row>
     <row r="19" spans="2:14" ht="214.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1485,25 +1488,25 @@
     </row>
     <row r="20" spans="2:14" ht="164.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>16</v>
@@ -1511,7 +1514,7 @@
       <c r="J20" s="7">
         <v>2</v>
       </c>
-      <c r="K20" s="13"/>
+      <c r="K20" s="15"/>
       <c r="L20" s="13"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>

</xml_diff>